<commit_message>
S03P23D105-10 | updated image & maked data
</commit_message>
<xml_diff>
--- a/back/fixtures/temp/branch.xlsx
+++ b/back/fixtures/temp/branch.xlsx
@@ -965,7 +965,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>

</xml_diff>